<commit_message>
finished first draft of intro!
</commit_message>
<xml_diff>
--- a/manuscript/tables_figures/table_variables.xlsx
+++ b/manuscript/tables_figures/table_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kteixeira/Dropbox (Smithsonian)/GitHub/SCBI-ForestGEO/McGregor_climate-sensitivity-variation/manuscript/tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58153EA-3720-3D47-BC96-8D9173A4FB70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECC64A9-908C-E440-83ED-B6AE0001CBF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7140" yWindow="2680" windowWidth="19440" windowHeight="15000" xr2:uid="{B3D4FDC9-1842-3C4E-B6CD-114DB37D495C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="57">
   <si>
     <t>variable</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>dry mass of a unit volume of fresh wood</t>
   </si>
 </sst>
 </file>
@@ -411,6 +414,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,54 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,7 +791,7 @@
   <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" activeCellId="2" sqref="I18:L18 I20:L21 I25:L26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -814,13 +817,13 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37" t="s">
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53" t="s">
         <v>37</v>
       </c>
     </row>
@@ -847,12 +850,12 @@
       <c r="I3" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="38"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="54"/>
     </row>
     <row r="4" spans="2:13" ht="22" customHeight="1">
       <c r="B4" s="22" t="s">
@@ -890,16 +893,16 @@
       <c r="H5" s="29">
         <v>1596</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="44">
         <v>0.87</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="45">
         <v>0</v>
       </c>
-      <c r="K5" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="51">
+      <c r="K5" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="47">
         <v>1.99</v>
       </c>
       <c r="M5" s="35" t="s">
@@ -1040,16 +1043,16 @@
       <c r="H11" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11" s="37">
         <v>31.92</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="38">
         <v>3.92</v>
       </c>
-      <c r="K11" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="44">
+      <c r="K11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="40">
         <v>134.19</v>
       </c>
       <c r="M11" s="30" t="s">
@@ -1076,16 +1079,16 @@
       <c r="H12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="40">
+      <c r="I12" s="36">
         <v>20.21</v>
       </c>
-      <c r="J12" s="45">
+      <c r="J12" s="41">
         <v>4.76</v>
       </c>
-      <c r="K12" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="47">
+      <c r="K12" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="43">
         <v>43.87</v>
       </c>
       <c r="M12" s="29" t="s">
@@ -1123,7 +1126,7 @@
       <c r="G14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="36">
         <v>31</v>
       </c>
       <c r="I14" s="29" t="s">
@@ -1149,7 +1152,7 @@
       <c r="G15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="36">
         <v>231</v>
       </c>
       <c r="I15" s="29" t="s">
@@ -1175,7 +1178,7 @@
       <c r="G16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="36">
         <v>224</v>
       </c>
       <c r="I16" s="29" t="s">
@@ -1201,7 +1204,7 @@
       <c r="G17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="36">
         <v>101</v>
       </c>
       <c r="I17" s="29" t="s">
@@ -1234,16 +1237,16 @@
       <c r="H18" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="36">
         <v>5.66</v>
       </c>
-      <c r="J18" s="45">
+      <c r="J18" s="41">
         <v>0</v>
       </c>
-      <c r="K18" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="47">
+      <c r="K18" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="43">
         <v>16</v>
       </c>
       <c r="M18" s="29" t="s">
@@ -1266,7 +1269,7 @@
       <c r="L19" s="25"/>
       <c r="M19" s="29"/>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" ht="28">
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>5</v>
@@ -1277,21 +1280,23 @@
       <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="11"/>
+      <c r="F20" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="41">
+      <c r="I20" s="37">
         <v>0.62</v>
       </c>
-      <c r="J20" s="42">
+      <c r="J20" s="38">
         <v>0.4</v>
       </c>
-      <c r="K20" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" s="44">
+      <c r="K20" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="40">
         <v>1.0900000000000001</v>
       </c>
       <c r="M20" s="30" t="s">
@@ -1314,16 +1319,16 @@
       <c r="H21" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I21" s="36">
         <v>48.69</v>
       </c>
-      <c r="J21" s="45">
+      <c r="J21" s="41">
         <v>30.68</v>
       </c>
-      <c r="K21" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" s="47">
+      <c r="K21" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="43">
         <v>75.8</v>
       </c>
       <c r="M21" s="29" t="s">
@@ -1345,7 +1350,7 @@
       <c r="G22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="41">
+      <c r="H22" s="37">
         <v>408</v>
       </c>
       <c r="I22" s="29" t="s">
@@ -1371,7 +1376,7 @@
       <c r="G23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="41">
+      <c r="H23" s="37">
         <v>31</v>
       </c>
       <c r="I23" s="29" t="s">
@@ -1397,7 +1402,7 @@
       <c r="G24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="41">
+      <c r="H24" s="37">
         <v>178</v>
       </c>
       <c r="I24" s="29" t="s">
@@ -1430,16 +1435,16 @@
       <c r="H25" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="36">
         <v>-2.39</v>
       </c>
-      <c r="J25" s="45">
+      <c r="J25" s="41">
         <v>-2.76</v>
       </c>
-      <c r="K25" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="L25" s="47">
+      <c r="K25" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="43">
         <v>-1.92</v>
       </c>
       <c r="M25" s="29" t="s">
@@ -1464,16 +1469,16 @@
       <c r="H26" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="I26" s="52">
+      <c r="I26" s="48">
         <v>13.06</v>
       </c>
-      <c r="J26" s="53">
+      <c r="J26" s="49">
         <v>8.52</v>
       </c>
-      <c r="K26" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="L26" s="55">
+      <c r="K26" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="51">
         <v>24.64</v>
       </c>
       <c r="M26" s="32" t="s">

</xml_diff>